<commit_message>
create function to estimate population size with competition
</commit_message>
<xml_diff>
--- a/temps_labos.xlsx
+++ b/temps_labos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t xml:space="preserve">Terminer exercice 2.2 et début exercice 2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminer exercice 2.3 et 2.4</t>
   </si>
 </sst>
 </file>
@@ -305,13 +308,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.43"/>
@@ -344,7 +347,7 @@
       </c>
       <c r="D2" s="3" t="n">
         <f aca="false">SUM(B2:B200)</f>
-        <v>40.65</v>
+        <v>42.65</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -532,6 +535,17 @@
       </c>
       <c r="C19" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="n">
+        <v>45524</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first draft labo 3 and create guide intro modelisation
</commit_message>
<xml_diff>
--- a/temps_labos.xlsx
+++ b/temps_labos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -113,6 +113,18 @@
   </si>
   <si>
     <t xml:space="preserve">Terminer exercice 2.3 et 2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure générale labo 3 et code function single_population_growth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminer exercice 1 du labo 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminer exercice 2,3,4,5,A,B du labo 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminer labo 3 et création guide introduction modélisation avec R</t>
   </si>
 </sst>
 </file>
@@ -308,13 +320,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.43"/>
@@ -347,7 +359,7 @@
       </c>
       <c r="D2" s="3" t="n">
         <f aca="false">SUM(B2:B200)</f>
-        <v>42.65</v>
+        <v>58.65</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -546,6 +558,50 @@
       </c>
       <c r="C20" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="n">
+        <v>45525</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="n">
+        <v>45526</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="n">
+        <v>45526</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="n">
+        <v>45526</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
terminer labo 3 et révision labo 1 et 2
</commit_message>
<xml_diff>
--- a/temps_labos.xlsx
+++ b/temps_labos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -125,16 +125,23 @@
   </si>
   <si>
     <t xml:space="preserve">Terminer labo 3 et création guide introduction modélisation avec R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer documents + corriger labo 1 et 2 et révision labo 1 et 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminer révision labo 2 et ajustement script </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-C0C]General"/>
     <numFmt numFmtId="166" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="167" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -222,7 +229,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -240,6 +247,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -320,13 +331,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.43"/>
@@ -359,7 +370,7 @@
       </c>
       <c r="D2" s="3" t="n">
         <f aca="false">SUM(B2:B200)</f>
-        <v>58.65</v>
+        <v>65.15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -602,6 +613,28 @@
       </c>
       <c r="C24" s="1" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="n">
+        <v>45527</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="n">
+        <v>45527</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deploy labo 1,2,3 on the shinyapp.io of uqar
</commit_message>
<xml_diff>
--- a/temps_labos.xlsx
+++ b/temps_labos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t xml:space="preserve">Terminer révision labo 2 et ajustement script </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Révision labo 3 et ajustement document labo 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rencontre Joël et deploiement shiny</t>
   </si>
 </sst>
 </file>
@@ -331,13 +337,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.43"/>
@@ -370,7 +376,7 @@
       </c>
       <c r="D2" s="3" t="n">
         <f aca="false">SUM(B2:B200)</f>
-        <v>65.15</v>
+        <v>73.15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -616,7 +622,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="n">
+      <c r="A25" s="4" t="n">
         <v>45527</v>
       </c>
       <c r="B25" s="1" t="n">
@@ -627,7 +633,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="n">
+      <c r="A26" s="4" t="n">
         <v>45527</v>
       </c>
       <c r="B26" s="1" t="n">
@@ -635,6 +641,28 @@
       </c>
       <c r="C26" s="1" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="n">
+        <v>45530</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="n">
+        <v>45530</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>